<commit_message>
Removing old Transport Profiles; TICC-248; TICC-249
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Transport profiles v8.4.xlsx
+++ b/work-in-progress/Peppol Code Lists - Transport profiles v8.4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407D7C61-655A-448B-9C88-B2D709FD4A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA00FFA7-9320-4E45-9967-DFF56EC11C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="37935" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3270" yWindow="1230" windowWidth="22695" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transport Profile" sheetId="5" r:id="rId1"/>
@@ -19,20 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Transport Profile'!$A$1:$G$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Profile ID</t>
   </si>
@@ -91,9 +82,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>deprecated</t>
-  </si>
-  <si>
     <t>active</t>
   </si>
   <si>
@@ -104,6 +92,12 @@
   </si>
   <si>
     <t>Removal Date</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>removed</t>
   </si>
 </sst>
 </file>
@@ -170,39 +164,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -614,19 +604,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="6"/>
+    <col min="1" max="1" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -639,17 +629,17 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -659,91 +649,106 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>1</v>
+      </c>
+      <c r="G2" s="11">
+        <v>45162</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="10">
+      <c r="E3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="8">
         <v>7</v>
+      </c>
+      <c r="G3" s="11">
+        <v>45162</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="9">
+      <c r="E4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="7">
         <v>3</v>
+      </c>
+      <c r="G4" s="11">
+        <v>45162</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>20</v>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>20</v>
+      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="11">
+        <v>45162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new "Comment" column at the end
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Transport profiles v8.4.xlsx
+++ b/work-in-progress/Peppol Code Lists - Transport profiles v8.4.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA00FFA7-9320-4E45-9967-DFF56EC11C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B3E249-3DB9-43EF-A81E-8832D2A19AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="1230" windowWidth="22695" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25215" yWindow="2460" windowWidth="22695" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transport Profile" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Transport Profile'!$A$1:$G$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Transport Profile'!$A$1:$H$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Profile ID</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>removed</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>TICC-248</t>
+  </si>
+  <si>
+    <t>TICC-249</t>
   </si>
 </sst>
 </file>
@@ -600,7 +609,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -619,7 +628,7 @@
     <col min="8" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -641,8 +650,11 @@
       <c r="G1" s="10" t="s">
         <v>22</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -664,8 +676,11 @@
       <c r="G2" s="11">
         <v>45162</v>
       </c>
+      <c r="H2" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -687,8 +702,11 @@
       <c r="G3" s="11">
         <v>45162</v>
       </c>
+      <c r="H3" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -710,8 +728,11 @@
       <c r="G4" s="11">
         <v>45162</v>
       </c>
+      <c r="H4" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -728,7 +749,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -750,9 +771,12 @@
       <c r="G6" s="11">
         <v>45162</v>
       </c>
+      <c r="H6" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G6" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H6" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>